<commit_message>
Moving from One Drive to GitHub
</commit_message>
<xml_diff>
--- a/2. 3D Printing/HyperCube_Evolution/files/HyperCube_Evolution_Configuration_v1.3.xlsx
+++ b/2. 3D Printing/HyperCube_Evolution/files/HyperCube_Evolution_Configuration_v1.3.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17927"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18067"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Scott Projects\3D Printing\CoreXY\Thingiverse Upload\Version 1.0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steve\OneDrive\Hobbies\3D Printing\designs\HyperCube_Evolution\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="162">
   <si>
     <t>Parameter name</t>
   </si>
@@ -380,9 +380,6 @@
     <t>bed_mounting_depth</t>
   </si>
   <si>
-    <t>Single</t>
-  </si>
-  <si>
     <t>bracket_size</t>
   </si>
   <si>
@@ -519,6 +516,12 @@
   </si>
   <si>
     <t>Part file is not available yet - Release TBA</t>
+  </si>
+  <si>
+    <t>Double</t>
+  </si>
+  <si>
+    <t>Done?</t>
   </si>
 </sst>
 </file>
@@ -686,7 +689,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -802,6 +805,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -809,7 +827,7 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="18" fillId="4" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -963,6 +981,24 @@
     <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -972,55 +1008,28 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="11" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1219,8 +1228,8 @@
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>151811</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1656,7 +1665,7 @@
       </c>
       <c r="C6" s="38">
         <f>ROUNDUP(G36/10,0)*10</f>
-        <v>380</v>
+        <v>480</v>
       </c>
       <c r="D6" s="39" t="s">
         <v>5</v>
@@ -1671,7 +1680,7 @@
       </c>
       <c r="C7" s="38">
         <f>ROUNDUP(G37/10,0)*10</f>
-        <v>370</v>
+        <v>470</v>
       </c>
       <c r="D7" s="39" t="s">
         <v>5</v>
@@ -1681,7 +1690,7 @@
       </c>
       <c r="G7" s="29">
         <f>Configuration!C15</f>
-        <v>200</v>
+        <v>300</v>
       </c>
     </row>
     <row r="8" spans="2:25" x14ac:dyDescent="0.25">
@@ -1711,7 +1720,7 @@
       </c>
       <c r="C9" s="38">
         <f>C24</f>
-        <v>214</v>
+        <v>328</v>
       </c>
       <c r="D9" s="39" t="s">
         <v>5</v>
@@ -1729,7 +1738,7 @@
       </c>
       <c r="C10" s="38">
         <f t="shared" ref="C10:C12" si="0">C25</f>
-        <v>214</v>
+        <v>328</v>
       </c>
       <c r="D10" s="39" t="s">
         <v>5</v>
@@ -1750,7 +1759,7 @@
       </c>
       <c r="C11" s="38">
         <f t="shared" si="0"/>
-        <v>210</v>
+        <v>325</v>
       </c>
       <c r="D11" s="39" t="s">
         <v>5</v>
@@ -1769,7 +1778,7 @@
       </c>
       <c r="C12" s="38">
         <f t="shared" si="0"/>
-        <v>210</v>
+        <v>325</v>
       </c>
       <c r="D12" s="39" t="s">
         <v>5</v>
@@ -1779,7 +1788,7 @@
       </c>
       <c r="G12" s="32">
         <f>C6-C5</f>
-        <v>350</v>
+        <v>450</v>
       </c>
       <c r="H12" s="27"/>
     </row>
@@ -1809,7 +1818,7 @@
       </c>
       <c r="C14" s="38">
         <f>MAX(180,IF(Configuration!$I$15="Double",Sheet1!$C$6-2*Sheet1!$C$5-5,$C$26-2*$C$28))</f>
-        <v>180</v>
+        <v>415</v>
       </c>
       <c r="D14" s="39" t="s">
         <v>5</v>
@@ -1825,7 +1834,7 @@
       </c>
       <c r="C15" s="38">
         <f>MAX(180,IF(Configuration!I15="Double",Sheet1!$C$27-2*Sheet1!$C$28,(ROUNDUP(($G$31-2.5+$G$8+$G$10+$G$17+$G$30/2+7.5)/10,0)*10)))</f>
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="D15" s="39" t="s">
         <v>5</v>
@@ -1837,7 +1846,7 @@
       </c>
       <c r="C16" s="38">
         <f>G30/2+G8+G10+G17/2</f>
-        <v>166.25</v>
+        <v>216.25</v>
       </c>
       <c r="D16" s="39" t="s">
         <v>5</v>
@@ -1861,12 +1870,12 @@
       </c>
       <c r="G17" s="29">
         <f>Configuration!C16</f>
-        <v>200</v>
+        <v>300</v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" s="37" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C18" s="38">
         <f>C28</f>
@@ -1933,7 +1942,7 @@
       </c>
       <c r="G22" s="29">
         <f>G7+G9+G21*2</f>
-        <v>345</v>
+        <v>445</v>
       </c>
       <c r="H22" s="27" t="s">
         <v>35</v>
@@ -1954,7 +1963,7 @@
       </c>
       <c r="G23" s="32">
         <f>C7-2*C5</f>
-        <v>310</v>
+        <v>410</v>
       </c>
       <c r="H23" s="27"/>
     </row>
@@ -1964,7 +1973,7 @@
       </c>
       <c r="C24" s="38">
         <f>VLOOKUP(Configuration!$F$15,Configuration!$M$6:'Configuration'!$Q$11,2,FALSE)</f>
-        <v>214</v>
+        <v>328</v>
       </c>
       <c r="D24" s="41" t="s">
         <v>5</v>
@@ -1977,7 +1986,7 @@
       </c>
       <c r="C25" s="38">
         <f>VLOOKUP(Configuration!$F$15,Configuration!$M$6:'Configuration'!$Q$11,3,FALSE)</f>
-        <v>214</v>
+        <v>328</v>
       </c>
       <c r="D25" s="41" t="s">
         <v>5</v>
@@ -1992,7 +2001,7 @@
       </c>
       <c r="C26" s="38">
         <f>VLOOKUP(Configuration!$F$15,Configuration!$M$6:'Configuration'!$Q$11,4,FALSE)</f>
-        <v>210</v>
+        <v>325</v>
       </c>
       <c r="D26" s="41" t="s">
         <v>5</v>
@@ -2014,7 +2023,7 @@
       </c>
       <c r="C27" s="38">
         <f>VLOOKUP(Configuration!$F$15,Configuration!$M$6:'Configuration'!$Q$11,5,FALSE)</f>
-        <v>210</v>
+        <v>325</v>
       </c>
       <c r="D27" s="41" t="s">
         <v>5</v>
@@ -2089,7 +2098,7 @@
       </c>
       <c r="G32" s="29">
         <f>IF(Configuration!I15="Double",Sheet1!C8-100,Sheet1!C8)</f>
-        <v>500</v>
+        <v>400</v>
       </c>
     </row>
     <row r="35" spans="6:10" x14ac:dyDescent="0.25">
@@ -2106,15 +2115,15 @@
       </c>
       <c r="G36" s="29">
         <f>IF(Configuration!I15="Double",MAX(I36:J36),Sheet1!I36)</f>
-        <v>375</v>
+        <v>475</v>
       </c>
       <c r="I36" s="64">
         <f>G22+C5</f>
-        <v>375</v>
+        <v>475</v>
       </c>
       <c r="J36" s="42">
         <f>$C$5+2*$G$31+2*$G$13+$C$24</f>
-        <v>348</v>
+        <v>462</v>
       </c>
     </row>
     <row r="37" spans="6:10" x14ac:dyDescent="0.25">
@@ -2123,15 +2132,15 @@
       </c>
       <c r="G37" s="29">
         <f>MAX(I37:J37)</f>
-        <v>363</v>
+        <v>463</v>
       </c>
       <c r="I37" s="42">
         <f>($G$18+$G$20/2-$G$10+$G$17+$G$10+$G$8+$G$30/2+$G$31+$C$5*2)</f>
-        <v>363</v>
+        <v>463</v>
       </c>
       <c r="J37" s="42">
         <f>($C$25+2*$C$5)</f>
-        <v>274</v>
+        <v>388</v>
       </c>
     </row>
     <row r="38" spans="6:10" x14ac:dyDescent="0.25">
@@ -2149,11 +2158,11 @@
       </c>
       <c r="I40" s="42">
         <f>$C$26-2*$C$28</f>
-        <v>180</v>
+        <v>295</v>
       </c>
       <c r="J40" s="42">
         <f>Sheet1!$C$6-2*Sheet1!$C$5-5</f>
-        <v>315</v>
+        <v>415</v>
       </c>
     </row>
     <row r="41" spans="6:10" x14ac:dyDescent="0.25">
@@ -2162,11 +2171,11 @@
       </c>
       <c r="I41" s="42">
         <f>(ROUNDUP(($G$31-2.5+$G$8+$G$10+$G$17+$G$30/2+7.5)/10,0)*10)</f>
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="J41" s="42">
         <f>Sheet1!$C$27-2*Sheet1!$C$28</f>
-        <v>180</v>
+        <v>295</v>
       </c>
     </row>
     <row r="43" spans="6:10" x14ac:dyDescent="0.25">
@@ -2179,11 +2188,11 @@
       </c>
       <c r="I43" s="42">
         <f>MAX(180,I40)+2*C28</f>
-        <v>210</v>
+        <v>325</v>
       </c>
       <c r="J43" s="42">
         <f>C26</f>
-        <v>210</v>
+        <v>325</v>
       </c>
     </row>
     <row r="44" spans="6:10" x14ac:dyDescent="0.25">
@@ -2196,11 +2205,11 @@
       </c>
       <c r="I44" s="42">
         <f>C27</f>
-        <v>210</v>
+        <v>325</v>
       </c>
       <c r="J44" s="42">
         <f>MAX(180,J41)+2*C28</f>
-        <v>210</v>
+        <v>325</v>
       </c>
     </row>
     <row r="45" spans="6:10" x14ac:dyDescent="0.25">
@@ -2224,8 +2233,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:V44"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView showGridLines="0" topLeftCell="A14" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2284,7 +2293,7 @@
         <v>94</v>
       </c>
       <c r="J3" s="56" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="L3" s="46"/>
       <c r="M3" s="24" t="s">
@@ -2294,14 +2303,14 @@
     <row r="4" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L4" s="46"/>
       <c r="M4" s="5"/>
-      <c r="N4" s="67" t="s">
+      <c r="N4" s="73" t="s">
         <v>69</v>
       </c>
-      <c r="O4" s="68"/>
-      <c r="P4" s="67" t="s">
+      <c r="O4" s="74"/>
+      <c r="P4" s="73" t="s">
         <v>63</v>
       </c>
-      <c r="Q4" s="69"/>
+      <c r="Q4" s="75"/>
     </row>
     <row r="5" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="L5" s="46"/>
@@ -2432,21 +2441,21 @@
         <v>97</v>
       </c>
       <c r="C15" s="21">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>5</v>
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="11" t="s">
-        <v>12</v>
+        <v>66</v>
       </c>
       <c r="G15" s="11" t="s">
         <v>68</v>
       </c>
       <c r="H15" s="3"/>
       <c r="I15" s="11" t="s">
-        <v>114</v>
+        <v>160</v>
       </c>
       <c r="J15" s="11" t="s">
         <v>68</v>
@@ -2461,7 +2470,7 @@
         <v>98</v>
       </c>
       <c r="C16" s="21">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>5</v>
@@ -2584,7 +2593,7 @@
       </c>
       <c r="C23" s="13">
         <f>Sheet1!C6-2*Sheet1!C5</f>
-        <v>320</v>
+        <v>420</v>
       </c>
       <c r="D23" s="13" t="s">
         <v>5</v>
@@ -2607,14 +2616,14 @@
       <c r="B24" s="53"/>
       <c r="C24" s="16">
         <f>Sheet1!C7-2*Sheet1!C5</f>
-        <v>310</v>
+        <v>410</v>
       </c>
       <c r="D24" s="16" t="s">
         <v>5</v>
       </c>
       <c r="E24" s="44">
         <f>IF(I15="Double",6,4)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F24" s="61" t="s">
         <v>85</v>
@@ -2645,14 +2654,14 @@
       </c>
       <c r="C26" s="16">
         <f>IF(I15="Double",Sheet1!C14,Sheet1!C14-2*Sheet1!C13)</f>
-        <v>140</v>
+        <v>415</v>
       </c>
       <c r="D26" s="16" t="s">
         <v>5</v>
       </c>
       <c r="E26" s="44">
         <f>IF(I15="Double",2,1)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F26" s="61" t="s">
         <v>87</v>
@@ -2663,7 +2672,7 @@
       <c r="B27" s="53"/>
       <c r="C27" s="16">
         <f>IF(I15="Double",Sheet1!C15-2*Sheet1!C13,Sheet1!C15)</f>
-        <v>300</v>
+        <v>255</v>
       </c>
       <c r="D27" s="16" t="s">
         <v>5</v>
@@ -2685,7 +2694,7 @@
       </c>
       <c r="C28" s="16">
         <f>Sheet1!G12</f>
-        <v>350</v>
+        <v>450</v>
       </c>
       <c r="D28" s="16" t="s">
         <v>5</v>
@@ -2707,7 +2716,7 @@
       </c>
       <c r="C29" s="16">
         <f>Sheet1!G23</f>
-        <v>310</v>
+        <v>410</v>
       </c>
       <c r="D29" s="16" t="s">
         <v>5</v>
@@ -2729,14 +2738,14 @@
       </c>
       <c r="C30" s="16">
         <f>Sheet1!G32</f>
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="D30" s="16" t="s">
         <v>5</v>
       </c>
       <c r="E30" s="44">
         <f>IF(I15="Double",4,2)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F30" s="61" t="s">
         <v>106</v>
@@ -2848,10 +2857,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:J42"/>
+  <dimension ref="B2:L42"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2861,15 +2870,15 @@
     <col min="3" max="3" width="16.28515625" customWidth="1"/>
     <col min="4" max="9" width="13.7109375" customWidth="1"/>
     <col min="10" max="10" width="41" customWidth="1"/>
-    <col min="11" max="11" width="2.85546875" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="73" t="s">
-        <v>154</v>
+      <c r="C2" s="67" t="s">
+        <v>153</v>
       </c>
       <c r="D2" s="58"/>
       <c r="E2" s="58"/>
@@ -2879,607 +2888,662 @@
       <c r="I2" s="58"/>
       <c r="J2" s="58"/>
     </row>
-    <row r="3" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="59" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="77" t="s">
-        <v>124</v>
-      </c>
-      <c r="D3" s="83" t="s">
+      <c r="C3" s="69" t="s">
+        <v>123</v>
+      </c>
+      <c r="D3" s="76" t="s">
+        <v>116</v>
+      </c>
+      <c r="E3" s="77"/>
+      <c r="F3" s="76" t="s">
+        <v>119</v>
+      </c>
+      <c r="G3" s="77"/>
+      <c r="H3" s="76" t="s">
+        <v>120</v>
+      </c>
+      <c r="I3" s="77"/>
+      <c r="J3" s="69" t="s">
+        <v>152</v>
+      </c>
+      <c r="K3" s="69" t="s">
+        <v>161</v>
+      </c>
+      <c r="L3" s="69"/>
+    </row>
+    <row r="4" spans="2:12" ht="27" x14ac:dyDescent="0.25">
+      <c r="B4" s="68" t="s">
+        <v>115</v>
+      </c>
+      <c r="C4" s="70"/>
+      <c r="D4" s="71" t="s">
         <v>117</v>
       </c>
-      <c r="E3" s="84"/>
-      <c r="F3" s="83" t="s">
-        <v>120</v>
-      </c>
-      <c r="G3" s="84"/>
-      <c r="H3" s="83" t="s">
+      <c r="E4" s="72" t="s">
+        <v>118</v>
+      </c>
+      <c r="F4" s="71" t="s">
+        <v>117</v>
+      </c>
+      <c r="G4" s="72" t="s">
+        <v>118</v>
+      </c>
+      <c r="H4" s="71" t="s">
         <v>121</v>
       </c>
-      <c r="I3" s="84"/>
-      <c r="J3" s="77" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="4" spans="2:10" ht="27" x14ac:dyDescent="0.25">
-      <c r="B4" s="76" t="s">
-        <v>116</v>
-      </c>
-      <c r="C4" s="78"/>
-      <c r="D4" s="81" t="s">
-        <v>118</v>
-      </c>
-      <c r="E4" s="85" t="s">
-        <v>119</v>
-      </c>
-      <c r="F4" s="81" t="s">
-        <v>118</v>
-      </c>
-      <c r="G4" s="85" t="s">
-        <v>119</v>
-      </c>
-      <c r="H4" s="81" t="s">
+      <c r="I4" s="72" t="s">
         <v>122</v>
       </c>
-      <c r="I4" s="85" t="s">
-        <v>123</v>
-      </c>
-      <c r="J4" s="78"/>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="J4" s="70"/>
+      <c r="K4" s="70"/>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B5" s="78"/>
       <c r="C5" s="79"/>
       <c r="D5" s="79"/>
-      <c r="E5" s="86"/>
+      <c r="E5" s="79"/>
       <c r="F5" s="79"/>
-      <c r="G5" s="86"/>
+      <c r="G5" s="79"/>
       <c r="H5" s="79"/>
-      <c r="I5" s="86"/>
-      <c r="J5" s="88"/>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>131</v>
+      <c r="I5" s="79"/>
+      <c r="J5" s="80"/>
+      <c r="K5" s="78"/>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B6" s="78" t="s">
+        <v>130</v>
       </c>
       <c r="C6" s="79">
         <v>1</v>
       </c>
       <c r="D6" s="79"/>
-      <c r="E6" s="86"/>
+      <c r="E6" s="79"/>
       <c r="F6" s="79"/>
-      <c r="G6" s="86"/>
+      <c r="G6" s="79"/>
       <c r="H6" s="79"/>
-      <c r="I6" s="86"/>
-      <c r="J6" s="88"/>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>125</v>
+      <c r="I6" s="79"/>
+      <c r="J6" s="80"/>
+      <c r="K6" s="78" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B7" s="78" t="s">
+        <v>124</v>
       </c>
       <c r="C7" s="79">
         <v>2</v>
       </c>
       <c r="D7" s="79"/>
-      <c r="E7" s="86"/>
+      <c r="E7" s="79"/>
       <c r="F7" s="79"/>
-      <c r="G7" s="86"/>
+      <c r="G7" s="79"/>
       <c r="H7" s="79"/>
-      <c r="I7" s="86"/>
-      <c r="J7" s="88"/>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>126</v>
+      <c r="I7" s="79"/>
+      <c r="J7" s="80"/>
+      <c r="K7" s="78" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B8" s="78" t="s">
+        <v>125</v>
       </c>
       <c r="C8" s="79">
         <v>4</v>
       </c>
       <c r="D8" s="79"/>
-      <c r="E8" s="86"/>
+      <c r="E8" s="79"/>
       <c r="F8" s="79"/>
-      <c r="G8" s="86"/>
+      <c r="G8" s="79"/>
       <c r="H8" s="79"/>
-      <c r="I8" s="86"/>
-      <c r="J8" s="88"/>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>127</v>
+      <c r="I8" s="79"/>
+      <c r="J8" s="80"/>
+      <c r="K8" s="78" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B9" s="78" t="s">
+        <v>126</v>
       </c>
       <c r="C9" s="79">
         <v>1</v>
       </c>
       <c r="D9" s="79"/>
-      <c r="E9" s="86"/>
+      <c r="E9" s="79"/>
       <c r="F9" s="79"/>
-      <c r="G9" s="86"/>
+      <c r="G9" s="79"/>
       <c r="H9" s="79"/>
-      <c r="I9" s="86"/>
-      <c r="J9" s="88"/>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>128</v>
+      <c r="I9" s="79"/>
+      <c r="J9" s="80"/>
+      <c r="K9" s="78"/>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B10" s="78" t="s">
+        <v>127</v>
       </c>
       <c r="C10" s="79">
         <v>1</v>
       </c>
       <c r="D10" s="79"/>
-      <c r="E10" s="86"/>
+      <c r="E10" s="79"/>
       <c r="F10" s="79"/>
-      <c r="G10" s="86"/>
+      <c r="G10" s="79"/>
       <c r="H10" s="79"/>
-      <c r="I10" s="86"/>
-      <c r="J10" s="88"/>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>129</v>
+      <c r="I10" s="79"/>
+      <c r="J10" s="80"/>
+      <c r="K10" s="78"/>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B11" s="78" t="s">
+        <v>128</v>
       </c>
       <c r="C11" s="79">
         <v>1</v>
       </c>
       <c r="D11" s="79"/>
-      <c r="E11" s="86"/>
+      <c r="E11" s="79"/>
       <c r="F11" s="79"/>
-      <c r="G11" s="86"/>
+      <c r="G11" s="79"/>
       <c r="H11" s="79"/>
-      <c r="I11" s="86"/>
-      <c r="J11" s="88"/>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>130</v>
+      <c r="I11" s="79"/>
+      <c r="J11" s="80"/>
+      <c r="K11" s="78"/>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B12" s="78" t="s">
+        <v>129</v>
       </c>
       <c r="C12" s="79" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D12" s="79"/>
-      <c r="E12" s="86"/>
+      <c r="E12" s="79"/>
       <c r="F12" s="79"/>
-      <c r="G12" s="86"/>
+      <c r="G12" s="79"/>
       <c r="H12" s="79"/>
-      <c r="I12" s="86"/>
-      <c r="J12" s="88"/>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>132</v>
+      <c r="I12" s="79"/>
+      <c r="J12" s="80"/>
+      <c r="K12" s="78"/>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B13" s="78" t="s">
+        <v>131</v>
       </c>
       <c r="C13" s="79">
         <v>2</v>
       </c>
       <c r="D13" s="79"/>
-      <c r="E13" s="86"/>
+      <c r="E13" s="79"/>
       <c r="F13" s="79"/>
-      <c r="G13" s="86"/>
+      <c r="G13" s="79"/>
       <c r="H13" s="79"/>
-      <c r="I13" s="86"/>
-      <c r="J13" s="88"/>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I13" s="79"/>
+      <c r="J13" s="80"/>
+      <c r="K13" s="78"/>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B14" s="78"/>
       <c r="C14" s="79"/>
       <c r="D14" s="79"/>
-      <c r="E14" s="86"/>
+      <c r="E14" s="79"/>
       <c r="F14" s="79"/>
-      <c r="G14" s="86"/>
+      <c r="G14" s="79"/>
       <c r="H14" s="79"/>
-      <c r="I14" s="86"/>
-      <c r="J14" s="88"/>
-    </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>146</v>
+      <c r="I14" s="79"/>
+      <c r="J14" s="80"/>
+      <c r="K14" s="78"/>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B15" s="78" t="s">
+        <v>145</v>
       </c>
       <c r="C15" s="79"/>
       <c r="D15" s="79"/>
-      <c r="E15" s="86"/>
+      <c r="E15" s="79"/>
       <c r="F15" s="79"/>
-      <c r="G15" s="86">
+      <c r="G15" s="79">
         <v>1</v>
       </c>
       <c r="H15" s="79"/>
-      <c r="I15" s="86"/>
-      <c r="J15" s="88"/>
-    </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>155</v>
+      <c r="I15" s="79"/>
+      <c r="J15" s="80"/>
+      <c r="K15" s="78"/>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B16" s="78" t="s">
+        <v>154</v>
       </c>
       <c r="C16" s="79"/>
       <c r="D16" s="79"/>
-      <c r="E16" s="86"/>
-      <c r="F16" s="90">
+      <c r="E16" s="79"/>
+      <c r="F16" s="81">
         <v>1</v>
       </c>
-      <c r="G16" s="86"/>
+      <c r="G16" s="79"/>
       <c r="H16" s="79"/>
-      <c r="I16" s="86"/>
-      <c r="J16" s="89" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>145</v>
+      <c r="I16" s="79"/>
+      <c r="J16" s="82" t="s">
+        <v>159</v>
+      </c>
+      <c r="K16" s="78"/>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B17" s="78" t="s">
+        <v>144</v>
       </c>
       <c r="C17" s="79"/>
       <c r="D17" s="79"/>
-      <c r="E17" s="86"/>
+      <c r="E17" s="79"/>
       <c r="F17" s="79"/>
-      <c r="G17" s="86">
+      <c r="G17" s="79">
         <v>1</v>
       </c>
       <c r="H17" s="79"/>
-      <c r="I17" s="86"/>
-      <c r="J17" s="88"/>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>156</v>
+      <c r="I17" s="79"/>
+      <c r="J17" s="80"/>
+      <c r="K17" s="78"/>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B18" s="78" t="s">
+        <v>155</v>
       </c>
       <c r="C18" s="79"/>
       <c r="D18" s="79"/>
-      <c r="E18" s="86"/>
-      <c r="F18" s="90">
+      <c r="E18" s="79"/>
+      <c r="F18" s="81">
         <v>1</v>
       </c>
-      <c r="G18" s="86"/>
+      <c r="G18" s="79"/>
       <c r="H18" s="79"/>
-      <c r="I18" s="86"/>
-      <c r="J18" s="89" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>148</v>
+      <c r="I18" s="79"/>
+      <c r="J18" s="82" t="s">
+        <v>159</v>
+      </c>
+      <c r="K18" s="78"/>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B19" s="78" t="s">
+        <v>147</v>
       </c>
       <c r="C19" s="79"/>
       <c r="D19" s="79"/>
-      <c r="E19" s="86"/>
+      <c r="E19" s="79"/>
       <c r="F19" s="79"/>
-      <c r="G19" s="86">
+      <c r="G19" s="79">
         <v>1</v>
       </c>
       <c r="H19" s="79"/>
-      <c r="I19" s="86"/>
-      <c r="J19" s="88"/>
-    </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>157</v>
+      <c r="I19" s="79"/>
+      <c r="J19" s="80"/>
+      <c r="K19" s="78"/>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B20" s="78" t="s">
+        <v>156</v>
       </c>
       <c r="C20" s="79"/>
       <c r="D20" s="79"/>
-      <c r="E20" s="86"/>
-      <c r="F20" s="90">
+      <c r="E20" s="79"/>
+      <c r="F20" s="81">
         <v>1</v>
       </c>
-      <c r="G20" s="86"/>
+      <c r="G20" s="79"/>
       <c r="H20" s="79"/>
-      <c r="I20" s="86"/>
-      <c r="J20" s="89" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>147</v>
+      <c r="I20" s="79"/>
+      <c r="J20" s="82" t="s">
+        <v>159</v>
+      </c>
+      <c r="K20" s="78"/>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B21" s="78" t="s">
+        <v>146</v>
       </c>
       <c r="C21" s="79"/>
       <c r="D21" s="79"/>
-      <c r="E21" s="86"/>
+      <c r="E21" s="79"/>
       <c r="F21" s="79"/>
-      <c r="G21" s="86">
+      <c r="G21" s="79">
         <v>1</v>
       </c>
       <c r="H21" s="79"/>
-      <c r="I21" s="86"/>
-      <c r="J21" s="88"/>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>158</v>
+      <c r="I21" s="79"/>
+      <c r="J21" s="80"/>
+      <c r="K21" s="78"/>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B22" s="78" t="s">
+        <v>157</v>
       </c>
       <c r="C22" s="79"/>
       <c r="D22" s="79"/>
-      <c r="E22" s="86"/>
-      <c r="F22" s="90">
+      <c r="E22" s="79"/>
+      <c r="F22" s="81">
         <v>1</v>
       </c>
-      <c r="G22" s="86"/>
+      <c r="G22" s="79"/>
       <c r="H22" s="79"/>
-      <c r="I22" s="86"/>
-      <c r="J22" s="89" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I22" s="79"/>
+      <c r="J22" s="82" t="s">
+        <v>159</v>
+      </c>
+      <c r="K22" s="78"/>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B23" s="78"/>
       <c r="C23" s="79"/>
       <c r="D23" s="79"/>
-      <c r="E23" s="86"/>
+      <c r="E23" s="79"/>
       <c r="F23" s="79"/>
-      <c r="G23" s="86"/>
+      <c r="G23" s="79"/>
       <c r="H23" s="79"/>
-      <c r="I23" s="86"/>
-      <c r="J23" s="88"/>
-    </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B24" s="71" t="s">
-        <v>134</v>
+      <c r="I23" s="79"/>
+      <c r="J23" s="80"/>
+      <c r="K23" s="78"/>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B24" s="83" t="s">
+        <v>133</v>
       </c>
       <c r="C24" s="79"/>
       <c r="D24" s="79"/>
-      <c r="E24" s="86"/>
+      <c r="E24" s="79"/>
       <c r="F24" s="79">
         <v>2</v>
       </c>
-      <c r="G24" s="86"/>
+      <c r="G24" s="79"/>
       <c r="H24" s="79"/>
-      <c r="I24" s="86"/>
-      <c r="J24" s="88"/>
-    </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B25" s="70" t="s">
-        <v>135</v>
+      <c r="I24" s="79"/>
+      <c r="J24" s="80"/>
+      <c r="K24" s="78"/>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B25" s="84" t="s">
+        <v>134</v>
       </c>
       <c r="C25" s="79"/>
       <c r="D25" s="79"/>
-      <c r="E25" s="86"/>
+      <c r="E25" s="79"/>
       <c r="F25" s="79"/>
-      <c r="G25" s="86">
+      <c r="G25" s="79">
         <v>2</v>
       </c>
       <c r="H25" s="79"/>
-      <c r="I25" s="86"/>
-      <c r="J25" s="88"/>
-    </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I25" s="79"/>
+      <c r="J25" s="80"/>
+      <c r="K25" s="78"/>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B26" s="78"/>
       <c r="C26" s="79"/>
       <c r="D26" s="79"/>
-      <c r="E26" s="86"/>
+      <c r="E26" s="79"/>
       <c r="F26" s="79"/>
-      <c r="G26" s="86"/>
+      <c r="G26" s="79"/>
       <c r="H26" s="79"/>
-      <c r="I26" s="86"/>
-      <c r="J26" s="88"/>
-    </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B27" s="72" t="s">
+      <c r="I26" s="79"/>
+      <c r="J26" s="80"/>
+      <c r="K26" s="78"/>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B27" s="84" t="s">
+        <v>135</v>
+      </c>
+      <c r="C27" s="79"/>
+      <c r="D27" s="85">
+        <v>2</v>
+      </c>
+      <c r="E27" s="79"/>
+      <c r="F27" s="85"/>
+      <c r="G27" s="79"/>
+      <c r="H27" s="79"/>
+      <c r="I27" s="79"/>
+      <c r="J27" s="80"/>
+      <c r="K27" s="78"/>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B28" s="84" t="s">
         <v>136</v>
       </c>
-      <c r="C27" s="79"/>
-      <c r="D27" s="82">
+      <c r="C28" s="79"/>
+      <c r="D28" s="85">
         <v>2</v>
       </c>
-      <c r="E27" s="86"/>
-      <c r="F27" s="82"/>
-      <c r="G27" s="86"/>
-      <c r="H27" s="79"/>
-      <c r="I27" s="86"/>
-      <c r="J27" s="88"/>
-    </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B28" s="72" t="s">
+      <c r="E28" s="79"/>
+      <c r="F28" s="79"/>
+      <c r="G28" s="85"/>
+      <c r="H28" s="79"/>
+      <c r="I28" s="79"/>
+      <c r="J28" s="80"/>
+      <c r="K28" s="78"/>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B29" s="84" t="s">
         <v>137</v>
-      </c>
-      <c r="C28" s="79"/>
-      <c r="D28" s="82">
-        <v>2</v>
-      </c>
-      <c r="E28" s="86"/>
-      <c r="F28" s="79"/>
-      <c r="G28" s="87"/>
-      <c r="H28" s="79"/>
-      <c r="I28" s="86"/>
-      <c r="J28" s="88"/>
-    </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B29" s="72" t="s">
-        <v>138</v>
       </c>
       <c r="C29" s="79"/>
       <c r="D29" s="79"/>
-      <c r="E29" s="87">
+      <c r="E29" s="85">
         <v>2</v>
       </c>
-      <c r="F29" s="82"/>
-      <c r="G29" s="86"/>
+      <c r="F29" s="85"/>
+      <c r="G29" s="79"/>
       <c r="H29" s="79"/>
-      <c r="I29" s="86"/>
-      <c r="J29" s="88"/>
-    </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B30" s="72" t="s">
-        <v>139</v>
+      <c r="I29" s="79"/>
+      <c r="J29" s="80"/>
+      <c r="K29" s="78"/>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B30" s="84" t="s">
+        <v>138</v>
       </c>
       <c r="C30" s="79"/>
       <c r="D30" s="79"/>
-      <c r="E30" s="87">
+      <c r="E30" s="85">
         <v>2</v>
       </c>
       <c r="F30" s="79"/>
-      <c r="G30" s="87"/>
+      <c r="G30" s="85"/>
       <c r="H30" s="79"/>
-      <c r="I30" s="86"/>
-      <c r="J30" s="88"/>
-    </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I30" s="79"/>
+      <c r="J30" s="80"/>
+      <c r="K30" s="78"/>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B31" s="78"/>
       <c r="C31" s="79"/>
       <c r="D31" s="79"/>
-      <c r="E31" s="86"/>
+      <c r="E31" s="79"/>
       <c r="F31" s="79"/>
-      <c r="G31" s="86"/>
+      <c r="G31" s="79"/>
       <c r="H31" s="79"/>
-      <c r="I31" s="86"/>
-      <c r="J31" s="88"/>
-    </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B32" s="74" t="s">
-        <v>140</v>
+      <c r="I31" s="79"/>
+      <c r="J31" s="80"/>
+      <c r="K31" s="78"/>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B32" s="84" t="s">
+        <v>139</v>
       </c>
       <c r="C32" s="79">
         <v>2</v>
       </c>
       <c r="D32" s="79"/>
-      <c r="E32" s="86"/>
+      <c r="E32" s="79"/>
       <c r="F32" s="79"/>
-      <c r="G32" s="86"/>
+      <c r="G32" s="79"/>
       <c r="H32" s="79"/>
-      <c r="I32" s="86"/>
-      <c r="J32" s="88"/>
-    </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B33" s="74" t="s">
-        <v>141</v>
+      <c r="I32" s="79"/>
+      <c r="J32" s="80"/>
+      <c r="K32" s="78"/>
+    </row>
+    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B33" s="84" t="s">
+        <v>140</v>
       </c>
       <c r="C33" s="79">
         <v>1</v>
       </c>
       <c r="D33" s="79"/>
-      <c r="E33" s="86"/>
+      <c r="E33" s="79"/>
       <c r="F33" s="79"/>
-      <c r="G33" s="86"/>
+      <c r="G33" s="79"/>
       <c r="H33" s="79"/>
-      <c r="I33" s="86"/>
-      <c r="J33" s="88"/>
-    </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I33" s="79"/>
+      <c r="J33" s="80"/>
+      <c r="K33" s="78"/>
+    </row>
+    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B34" s="78"/>
       <c r="C34" s="79"/>
       <c r="D34" s="79"/>
-      <c r="E34" s="86"/>
+      <c r="E34" s="79"/>
       <c r="F34" s="79"/>
-      <c r="G34" s="86"/>
+      <c r="G34" s="79"/>
       <c r="H34" s="79"/>
-      <c r="I34" s="86"/>
-      <c r="J34" s="88"/>
-    </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B35" s="75" t="s">
-        <v>142</v>
+      <c r="I34" s="79"/>
+      <c r="J34" s="80"/>
+      <c r="K34" s="78"/>
+    </row>
+    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B35" s="84" t="s">
+        <v>141</v>
       </c>
       <c r="C35" s="79"/>
       <c r="D35" s="79"/>
-      <c r="E35" s="86"/>
+      <c r="E35" s="79"/>
       <c r="F35" s="79"/>
-      <c r="G35" s="86"/>
+      <c r="G35" s="79"/>
       <c r="H35" s="79">
         <v>2</v>
       </c>
-      <c r="I35" s="86">
+      <c r="I35" s="79">
         <v>4</v>
       </c>
-      <c r="J35" s="88"/>
-    </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B36" s="75" t="s">
-        <v>150</v>
-      </c>
-      <c r="C36" s="80"/>
-      <c r="D36" s="80"/>
-      <c r="E36" s="53"/>
-      <c r="F36" s="80"/>
-      <c r="G36" s="53"/>
+      <c r="J35" s="80"/>
+      <c r="K35" s="78"/>
+    </row>
+    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B36" s="84" t="s">
+        <v>149</v>
+      </c>
+      <c r="C36" s="78"/>
+      <c r="D36" s="78"/>
+      <c r="E36" s="78"/>
+      <c r="F36" s="78"/>
+      <c r="G36" s="78"/>
       <c r="H36" s="79">
         <v>2</v>
       </c>
-      <c r="I36" s="86">
+      <c r="I36" s="79">
         <v>2</v>
       </c>
-      <c r="J36" s="88"/>
-    </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B37" s="75" t="s">
-        <v>149</v>
-      </c>
-      <c r="C37" s="80"/>
-      <c r="D37" s="80"/>
-      <c r="E37" s="53"/>
-      <c r="F37" s="80"/>
-      <c r="G37" s="53"/>
+      <c r="J36" s="80"/>
+      <c r="K36" s="78"/>
+    </row>
+    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B37" s="84" t="s">
+        <v>148</v>
+      </c>
+      <c r="C37" s="78"/>
+      <c r="D37" s="78"/>
+      <c r="E37" s="78"/>
+      <c r="F37" s="78"/>
+      <c r="G37" s="78"/>
       <c r="H37" s="79">
         <v>2</v>
       </c>
-      <c r="I37" s="86">
+      <c r="I37" s="79">
         <v>2</v>
       </c>
-      <c r="J37" s="88"/>
-    </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B38" s="75" t="s">
-        <v>152</v>
+      <c r="J37" s="80"/>
+      <c r="K37" s="78"/>
+    </row>
+    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B38" s="84" t="s">
+        <v>151</v>
       </c>
       <c r="C38" s="79"/>
       <c r="D38" s="79"/>
-      <c r="E38" s="86"/>
+      <c r="E38" s="79"/>
       <c r="F38" s="79"/>
-      <c r="G38" s="86"/>
+      <c r="G38" s="79"/>
       <c r="H38" s="79"/>
-      <c r="I38" s="86">
+      <c r="I38" s="79">
         <v>2</v>
       </c>
-      <c r="J38" s="88"/>
-    </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B39" s="75" t="s">
-        <v>151</v>
+      <c r="J38" s="80"/>
+      <c r="K38" s="78"/>
+    </row>
+    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B39" s="84" t="s">
+        <v>150</v>
       </c>
       <c r="C39" s="79"/>
       <c r="D39" s="79"/>
-      <c r="E39" s="86"/>
+      <c r="E39" s="79"/>
       <c r="F39" s="79"/>
-      <c r="G39" s="86"/>
+      <c r="G39" s="79"/>
       <c r="H39" s="79"/>
-      <c r="I39" s="86">
+      <c r="I39" s="79">
         <v>2</v>
       </c>
-      <c r="J39" s="88"/>
-    </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B40" s="75"/>
+      <c r="J39" s="80"/>
+      <c r="K39" s="78"/>
+    </row>
+    <row r="40" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B40" s="84"/>
       <c r="C40" s="79"/>
       <c r="D40" s="79"/>
-      <c r="E40" s="86"/>
+      <c r="E40" s="79"/>
       <c r="F40" s="79"/>
-      <c r="G40" s="86"/>
+      <c r="G40" s="79"/>
       <c r="H40" s="79"/>
-      <c r="I40" s="86"/>
-      <c r="J40" s="88"/>
-    </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B41" s="75" t="s">
-        <v>143</v>
-      </c>
-      <c r="C41" s="80"/>
-      <c r="D41" s="80"/>
-      <c r="E41" s="53"/>
-      <c r="F41" s="80"/>
-      <c r="G41" s="53"/>
+      <c r="I40" s="79"/>
+      <c r="J40" s="80"/>
+      <c r="K40" s="78"/>
+    </row>
+    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B41" s="84" t="s">
+        <v>142</v>
+      </c>
+      <c r="C41" s="78"/>
+      <c r="D41" s="78"/>
+      <c r="E41" s="78"/>
+      <c r="F41" s="78"/>
+      <c r="G41" s="78"/>
       <c r="H41" s="79">
         <v>1</v>
       </c>
-      <c r="I41" s="86">
+      <c r="I41" s="79">
         <v>2</v>
       </c>
-      <c r="J41" s="88"/>
-    </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B42" s="75" t="s">
-        <v>144</v>
-      </c>
-      <c r="C42" s="80"/>
-      <c r="D42" s="80"/>
-      <c r="E42" s="80"/>
-      <c r="F42" s="80"/>
-      <c r="G42" s="53"/>
+      <c r="J41" s="80"/>
+      <c r="K41" s="78"/>
+    </row>
+    <row r="42" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B42" s="84" t="s">
+        <v>143</v>
+      </c>
+      <c r="C42" s="78"/>
+      <c r="D42" s="78"/>
+      <c r="E42" s="78"/>
+      <c r="F42" s="78"/>
+      <c r="G42" s="78"/>
       <c r="H42" s="79">
         <v>1</v>
       </c>
-      <c r="I42" s="86">
+      <c r="I42" s="79">
         <v>2</v>
       </c>
-      <c r="J42" s="88"/>
+      <c r="J42" s="80"/>
+      <c r="K42" s="78"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>